<commit_message>
menambahkan fitur export pajak kelurahan
</commit_message>
<xml_diff>
--- a/resources/excel/templatexcel.xlsx
+++ b/resources/excel/templatexcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\app-reminder\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\app-reminder-billing\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5B466A-F0DF-4D91-BDFC-C97C0668879A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77685A4B-A53C-47B2-B3A8-A56CF7043863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E93310B-EC91-401E-9442-573EEEDD4E0B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>nama user</t>
   </si>
@@ -51,10 +51,19 @@
     <t>no faktur</t>
   </si>
   <si>
-    <t>NOO1212</t>
-  </si>
-  <si>
-    <t>Ifkar H</t>
+    <t>RSU PKU MUHAMMADIYAH DELANGGU</t>
+  </si>
+  <si>
+    <t>FOCUS INDEPENDEN SCHOOL</t>
+  </si>
+  <si>
+    <t>PT Vinsa Mandiri Utama III</t>
+  </si>
+  <si>
+    <t>YAYASAN LEMBAGA ELTI GRAMEDIA</t>
+  </si>
+  <si>
+    <t>SMA AL AZHAR SYIFA BUDI SURAKARTA</t>
   </si>
 </sst>
 </file>
@@ -406,13 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC9C9B4-F7FF-4CE4-AC3D-353CABA0F56F}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -432,20 +444,88 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>100082444248363</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>2020000</v>
+      </c>
+      <c r="D2">
+        <v>1819820</v>
+      </c>
+      <c r="E2">
+        <v>200180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100082444248365</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>300000</v>
-      </c>
-      <c r="D2">
-        <v>150000</v>
-      </c>
-      <c r="E2">
-        <v>150000</v>
+      <c r="C3">
+        <v>1400000</v>
+      </c>
+      <c r="D3">
+        <v>1261261</v>
+      </c>
+      <c r="E3">
+        <v>138739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100082444248367</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1200000</v>
+      </c>
+      <c r="D4">
+        <v>1081081</v>
+      </c>
+      <c r="E4">
+        <v>118919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100082444248368</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1200000</v>
+      </c>
+      <c r="D5">
+        <v>1081081</v>
+      </c>
+      <c r="E5">
+        <v>118919</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100082444248369</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>1200000</v>
+      </c>
+      <c r="D6">
+        <v>1081081</v>
+      </c>
+      <c r="E6">
+        <v>118919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>